<commit_message>
Added techlistic base, pages, tests
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,18 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A80E6B63-8C60-43AD-8A35-C3E2211066F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CBD85B44-4594-4AD9-BB94-798080685074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{9357FE9C-01F2-4E6A-BB47-050F08CB45AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{9357FE9C-01F2-4E6A-BB47-050F08CB45AE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="LeftForm" sheetId="1" r:id="rId1"/>
+    <sheet name="RightForm" sheetId="2" r:id="rId2"/>
+    <sheet name="TechlisticForm" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M18"/>
+  <oleSize ref="A1:J14"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -95,13 +96,86 @@
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Name </t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Years of Exp</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Profession</t>
+  </si>
+  <si>
+    <t>Automation Tools</t>
+  </si>
+  <si>
+    <t>Continents</t>
+  </si>
+  <si>
+    <t>Selenium Commands</t>
+  </si>
+  <si>
+    <t>File Path</t>
+  </si>
+  <si>
+    <t>Actual Resuts</t>
+  </si>
+  <si>
+    <t>Imran</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>16-07-25</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>WebElement Commands</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>mno</t>
+  </si>
+  <si>
+    <t>16-07-26</t>
+  </si>
+  <si>
+    <t>All fields filled, Submit button clicked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selenium </t>
+  </si>
+  <si>
+    <t>C:\Users\DELL\Desktop\dummy.txt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +187,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -462,16 +542,16 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.42578125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="22.5703125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.140625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -492,70 +572,70 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>14</v>
       </c>
     </row>
@@ -569,17 +649,17 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.42578125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.5703125"/>
+    <col min="3" max="3" customWidth="true" width="17.5703125"/>
+    <col min="4" max="4" customWidth="true" width="19.7109375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -600,74 +680,270 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CF479E2-70F2-4A96-944F-CEEC52E0F9C4}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="12.28515625"/>
+    <col min="2" max="2" customWidth="true" width="12.0"/>
+    <col min="3" max="3" customWidth="true" width="9.140625"/>
+    <col min="4" max="4" customWidth="true" width="15.5703125"/>
+    <col min="5" max="5" customWidth="true" width="10.28515625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.85546875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.5703125"/>
+    <col min="8" max="8" customWidth="true" width="13.85546875"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="23.28515625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="39.5703125"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="35.140625"/>
+    <col min="12" max="12" customWidth="true" width="16.28515625"/>
+    <col min="13" max="13" customWidth="true" width="9.85546875"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="D2" s="0">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="D3" s="0">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="D4" s="0">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="M4" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update TestData.xlsx with latest OrangeHRM test data
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,19 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CBD85B44-4594-4AD9-BB94-798080685074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{DE2707C8-128A-4DFE-BD09-ACFA8318AD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{9357FE9C-01F2-4E6A-BB47-050F08CB45AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{9357FE9C-01F2-4E6A-BB47-050F08CB45AE}"/>
   </bookViews>
   <sheets>
     <sheet name="LeftForm" sheetId="1" r:id="rId1"/>
     <sheet name="RightForm" sheetId="2" r:id="rId2"/>
     <sheet name="TechlisticForm" sheetId="3" r:id="rId3"/>
+    <sheet name="OrangeHRM_LoginForm" sheetId="4" r:id="rId4"/>
+    <sheet name="ParaBank_RegistartionForm" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J14"/>
+  <oleSize ref="A1:I13"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -168,13 +170,79 @@
   </si>
   <si>
     <t>C:\Users\DELL\Desktop\dummy.txt</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status </t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>incorrectpassword</t>
+  </si>
+  <si>
+    <t>Invalid Credentials</t>
+  </si>
+  <si>
+    <t>Invalid credentials</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>Phone #</t>
+  </si>
+  <si>
+    <t>SSN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username </t>
+  </si>
+  <si>
+    <t>Confirm</t>
+  </si>
+  <si>
+    <t>Lahore</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>secret123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your account was created successfully. You are now logged in.
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -218,11 +286,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,11 +624,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="7.42578125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="22.5703125"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.140625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.28515625"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -572,70 +649,70 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -655,11 +732,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="7.42578125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.5703125"/>
-    <col min="3" max="3" customWidth="true" width="17.5703125"/>
-    <col min="4" max="4" customWidth="true" width="19.7109375"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.140625"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -680,70 +757,70 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -758,24 +835,24 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J4"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.28515625"/>
-    <col min="2" max="2" customWidth="true" width="12.0"/>
-    <col min="3" max="3" customWidth="true" width="9.140625"/>
-    <col min="4" max="4" customWidth="true" width="15.5703125"/>
-    <col min="5" max="5" customWidth="true" width="10.28515625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.85546875"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.5703125"/>
-    <col min="8" max="8" customWidth="true" width="13.85546875"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="23.28515625"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="39.5703125"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="35.140625"/>
-    <col min="12" max="12" customWidth="true" width="16.28515625"/>
-    <col min="13" max="13" customWidth="true" width="9.85546875"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.85546875" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -820,125 +897,125 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="0">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>44</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>46</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>38</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>39</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>47</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="K2" t="s">
         <v>43</v>
       </c>
-      <c r="L2" t="s" s="0">
+      <c r="L2" t="s">
         <v>43</v>
       </c>
-      <c r="M2" t="s" s="0">
+      <c r="M2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="0">
+      <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>37</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>45</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="G3" t="s">
         <v>46</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>38</v>
       </c>
-      <c r="I3" t="s" s="0">
+      <c r="I3" t="s">
         <v>39</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="J3" t="s">
         <v>47</v>
       </c>
-      <c r="K3" t="s" s="0">
+      <c r="K3" t="s">
         <v>43</v>
       </c>
-      <c r="L3" t="s" s="0">
+      <c r="L3" t="s">
         <v>43</v>
       </c>
-      <c r="M3" t="s" s="0">
+      <c r="M3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="0">
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>42</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>45</v>
       </c>
-      <c r="G4" t="s" s="0">
+      <c r="G4" t="s">
         <v>46</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H4" t="s">
         <v>38</v>
       </c>
-      <c r="I4" t="s" s="0">
+      <c r="I4" t="s">
         <v>39</v>
       </c>
-      <c r="J4" t="s" s="0">
+      <c r="J4" t="s">
         <v>47</v>
       </c>
-      <c r="K4" t="s" s="0">
+      <c r="K4" t="s">
         <v>43</v>
       </c>
-      <c r="L4" t="s" s="0">
+      <c r="L4" t="s">
         <v>43</v>
       </c>
-      <c r="M4" t="s" s="0">
+      <c r="M4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -946,4 +1023,194 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6B11A6-5BC3-4629-A744-5D540E81A471}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D526D43E-15B3-44DE-B056-64F0C7D274F1}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="4">
+        <v>13144</v>
+      </c>
+      <c r="G2" s="4">
+        <v>13141424</v>
+      </c>
+      <c r="H2" s="4">
+        <v>2222345</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update TestData.xlsx with latest ParaBank test data
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{DE2707C8-128A-4DFE-BD09-ACFA8318AD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{EFE12683-37B0-45D1-8AEE-DD1D96BE0C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{9357FE9C-01F2-4E6A-BB47-050F08CB45AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="5" xr2:uid="{9357FE9C-01F2-4E6A-BB47-050F08CB45AE}"/>
   </bookViews>
   <sheets>
     <sheet name="LeftForm" sheetId="1" r:id="rId1"/>
     <sheet name="RightForm" sheetId="2" r:id="rId2"/>
     <sheet name="TechlisticForm" sheetId="3" r:id="rId3"/>
     <sheet name="OrangeHRM_LoginForm" sheetId="4" r:id="rId4"/>
-    <sheet name="ParaBank_RegistartionForm" sheetId="5" r:id="rId5"/>
+    <sheet name="ParaBank_RegistrationForm" sheetId="5" r:id="rId5"/>
+    <sheet name="ParaBank_LoginForm" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <oleSize ref="A1:I13"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -237,6 +238,24 @@
   <si>
     <t xml:space="preserve">Your account was created successfully. You are now logged in.
 </t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Your account was created successfully. You are now logged in.</t>
+  </si>
+  <si>
+    <t>wrongpassword</t>
+  </si>
+  <si>
+    <t>The username and password could not be verified.</t>
+  </si>
+  <si>
+    <t>Login Success</t>
   </si>
 </sst>
 </file>
@@ -834,7 +853,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
@@ -1028,7 +1047,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6B11A6-5BC3-4629-A744-5D540E81A471}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -1044,7 +1063,7 @@
     <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -1061,7 +1080,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1078,7 +1097,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1107,7 +1126,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,10 +1193,10 @@
     </row>
     <row r="2" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>7</v>
@@ -1198,7 +1217,7 @@
         <v>2222345</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>68</v>
@@ -1208,6 +1227,86 @@
       </c>
       <c r="L2" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="M2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7270622-9E24-4265-ADE6-EA3EF64E5593}">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ParaBank base, pages, tests and updated Excel data
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\git\repository\automation.com\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{806DB3A1-D576-4FB1-80CD-3CD62FFDBA04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{85988A8A-5850-47FD-B305-B391B34890D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7875" firstSheet="4" activeTab="4" xr2:uid="{9357FE9C-01F2-4E6A-BB47-050F08CB45AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="4" xr2:uid="{9357FE9C-01F2-4E6A-BB47-050F08CB45AE}"/>
   </bookViews>
   <sheets>
     <sheet name="LeftForm" sheetId="1" r:id="rId1"/>
@@ -21,6 +16,7 @@
     <sheet name="ParaBank_LoginForm" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:L8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -250,6 +246,9 @@
     <t>Beta</t>
   </si>
   <si>
+    <t>Your account was created successfully. You are now logged in.</t>
+  </si>
+  <si>
     <t>wrongpassword</t>
   </si>
   <si>
@@ -257,11 +256,6 @@
   </si>
   <si>
     <t>Login Success</t>
-  </si>
-  <si>
-    <t>Your account was created 
-successfully. You are now 
-logged in.</t>
   </si>
 </sst>
 </file>
@@ -1131,7 +1125,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
@@ -1234,11 +1228,11 @@
       <c r="L2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>75</v>
+      <c r="M2" t="s">
+        <v>72</v>
       </c>
       <c r="N2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1289,10 +1283,10 @@
         <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
@@ -1303,13 +1297,13 @@
         <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>

</xml_diff>